<commit_message>
Quite a few changes I have now performed the imputation for missing SDs and means I've transformed SEs to SDs I've also calculated mean sds for each time point and arm for med studies using CDRS, so that this average value can be used when all SDs are missing for a study
</commit_message>
<xml_diff>
--- a/columns_with_missing_values_updated.xlsx
+++ b/columns_with_missing_values_updated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/rejucbu_ucl_ac_uk/Documents/Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents/apples_oranges/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\OneDrive - University College London\Response to Psychological and Pharmacological Treatment for Depression in Children and Adolescents\apples_oranges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{5D645470-5711-4317-87BC-E002C69CDA0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD47D63-ED62-4DB8-8ECC-A5CDA1ED7325}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="8_{5D645470-5711-4317-87BC-E002C69CDA0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2C333E1-EB66-4C7A-86BA-534BF0DDA77C}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="34160" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="500" windowWidth="18080" windowHeight="5890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="207">
   <si>
     <t>study</t>
   </si>
@@ -574,9 +574,6 @@
     <t>nA</t>
   </si>
   <si>
-    <t>we have only changes score, see Cipriani, probably use other study to impute</t>
-  </si>
-  <si>
     <t xml:space="preserve">use  cdrs changes score to calculate post-test means, use baseline SD to impute the missing post SD, and transform the SE to SD. </t>
   </si>
   <si>
@@ -598,18 +595,6 @@
     <t>This study does not appear in Cuijpers' MA because it does not report on a continuous outcome variable.</t>
   </si>
   <si>
-    <t xml:space="preserve">Only post-test means are available. No baseline means, changes scores, or sds available. Cipriani has change scores, not sure where these came from. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to derive SDs from SEs. No baseline or post-test means or SDs are reported and cannot be computed. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Need to go to original study and input change scores and baseline means and SDs. Not sure why this wasn't included in Cuijpers' dataset/list of included studies. </t>
-  </si>
-  <si>
-    <t>Does not report post test means or SDs. The only mention of change scores is "both reduced by 16 points". Possibly not usable?</t>
-  </si>
-  <si>
     <t>Not included in Cuijpers MA. Neither post-test means nor change scores are reported. Only slopes for linear model reported.</t>
   </si>
   <si>
@@ -631,14 +616,38 @@
     <t>No post test means or SDs reported. No change scores reported. Can try to derive post-test means using Cipriani data. Can impute post SDs using baseline SDs.</t>
   </si>
   <si>
-    <t xml:space="preserve">Post test mean can be derived from change score. No SDs reported. </t>
+    <t>we have only changes scores, neither baseline or post test means. Probably use other study to impute SDs?</t>
+  </si>
+  <si>
+    <t>Only post-test means are available. No baseline means, changes scores, or sds available. Cipriani has change scores, not sure where these came from. Can use these to compute baseline means. Borrow SDs from other studies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to derive change score SDs from SEs. No baseline or post-test means are reported and cannot be computed. Can take SDs from another study. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does not report post test means or SDs. Post SDs can be imputed using baseline SDs. The only mention of change scores is "both reduced by 16 points". Possibly not usable? Actually Cipriani has some change scores reported, which we could try to use to impute missing post means. The baseline means are also reported in a suspicious manner (both groups had means of 30 +/- 5). </t>
+  </si>
+  <si>
+    <t>Post test mean can be derived from change score. No SDs reported. Take from another study.</t>
+  </si>
+  <si>
+    <t>Does not report on a continuous outcome measure. Not included in Cuipers MA.</t>
+  </si>
+  <si>
+    <t>Does not report any baseline scores or change scores.</t>
+  </si>
+  <si>
+    <t>This study does not appear in Cuijpers' MA - in his dataset it is characterised as using "another statistic" rather than means/sds. However, going back to the original paper, I can see that we could extract pre and post means if we wish to. Can see baseline but not post SDs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to go to original study and input baseline means and SDs. There are also change scores in Cuijpers' dataset. This study wasn't included in Cuijpers' dataset/list of included studies because it does not report a continuous post-test outcome. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -652,8 +661,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,6 +677,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,12 +748,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,11 +1058,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1212,7 +1253,9 @@
       <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>60</v>
@@ -1289,7 +1332,9 @@
       <c r="B3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>65</v>
@@ -2054,7 +2099,7 @@
       <c r="B10" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>182</v>
       </c>
       <c r="D10" s="2">
@@ -2307,8 +2352,8 @@
       <c r="B13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>198</v>
+      <c r="C13" s="5" t="s">
+        <v>193</v>
       </c>
       <c r="D13" s="2">
         <v>12</v>
@@ -2602,8 +2647,8 @@
       <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>184</v>
+      <c r="C16" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="D16" s="2">
         <v>19</v>
@@ -2872,7 +2917,7 @@
         <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D19" s="2">
         <v>22</v>
@@ -3090,7 +3135,7 @@
         <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D21" s="2">
         <v>27</v>
@@ -3205,7 +3250,7 @@
         <v>102</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D22" s="2">
         <v>26</v>
@@ -3322,7 +3367,7 @@
         <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D23" s="2">
         <v>24</v>
@@ -3455,7 +3500,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D24" s="2">
         <v>25</v>
@@ -3588,7 +3633,7 @@
         <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D25" s="2">
         <v>28</v>
@@ -3816,7 +3861,7 @@
         <v>70</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D27" s="2">
         <v>30</v>
@@ -3937,7 +3982,7 @@
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D28" s="2">
         <v>31</v>
@@ -4056,7 +4101,7 @@
         <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D29" s="2">
         <v>32</v>
@@ -4269,14 +4314,14 @@
       <c r="BG30" s="2"/>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D31" s="2">
         <v>40</v>
@@ -4360,14 +4405,14 @@
       <c r="BG31" s="2"/>
     </row>
     <row r="32" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="6" t="s">
         <v>119</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>120</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D32" s="2">
         <v>41</v>
@@ -4761,7 +4806,7 @@
         <v>133</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D36" s="2">
         <v>53</v>
@@ -4858,7 +4903,7 @@
         <v>137</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
@@ -5033,14 +5078,14 @@
       <c r="BG38" s="2"/>
     </row>
     <row r="39" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>192</v>
+      <c r="C39" s="8" t="s">
+        <v>199</v>
       </c>
       <c r="D39" s="2">
         <v>1</v>
@@ -5132,14 +5177,14 @@
       <c r="BG39" s="2"/>
     </row>
     <row r="40" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>189</v>
+      <c r="C40" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="D40" s="2">
         <v>2</v>
@@ -5229,14 +5274,14 @@
       <c r="BG40" s="2"/>
     </row>
     <row r="41" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="6" t="s">
         <v>145</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>193</v>
+      <c r="C41" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="D41" s="2">
         <v>59</v>
@@ -5334,7 +5379,7 @@
       <c r="BG41" s="2"/>
     </row>
     <row r="42" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="6" t="s">
         <v>145</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -5433,14 +5478,14 @@
       <c r="BG42" s="2"/>
     </row>
     <row r="43" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="6" t="s">
         <v>147</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>191</v>
+      <c r="C43" s="9" t="s">
+        <v>205</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
@@ -5522,14 +5567,14 @@
       <c r="BG43" s="2"/>
     </row>
     <row r="44" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="6" t="s">
         <v>152</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>194</v>
+      <c r="C44" s="9" t="s">
+        <v>206</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2" t="s">
@@ -5603,14 +5648,14 @@
       <c r="BG44" s="2"/>
     </row>
     <row r="45" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="6" t="s">
         <v>156</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>199</v>
+      <c r="C45" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
@@ -5684,14 +5729,14 @@
       <c r="BG45" s="2"/>
     </row>
     <row r="46" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="7" t="s">
         <v>158</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>195</v>
+      <c r="C46" s="4" t="s">
+        <v>201</v>
       </c>
       <c r="D46" s="2">
         <v>63</v>
@@ -5899,7 +5944,7 @@
         <v>163</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D48" s="2">
         <v>64</v>
@@ -6106,14 +6151,14 @@
       <c r="BG49" s="2"/>
     </row>
     <row r="50" spans="1:59" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="7" t="s">
         <v>162</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D50" s="2">
         <v>66</v>
@@ -6330,8 +6375,8 @@
       <c r="B52" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>203</v>
+      <c r="C52" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="D52" s="2">
         <v>68</v>
@@ -6549,7 +6594,7 @@
         <v>172</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
@@ -6718,8 +6763,8 @@
       <c r="B56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>197</v>
+      <c r="C56" s="10" t="s">
+        <v>192</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
@@ -6830,6 +6875,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>